<commit_message>
fix Perhitungan BHP dan halaman cetak
</commit_message>
<xml_diff>
--- a/public/excel/export_barang_persediaan.xlsx
+++ b/public/excel/export_barang_persediaan.xlsx
@@ -86,30 +86,30 @@
     <t>Sarung tangan sterill size 7</t>
   </si>
   <si>
+    <t>Asam mefenamat</t>
+  </si>
+  <si>
+    <t>Charm wings</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hansaplast </t>
   </si>
   <si>
+    <t>Hansaplast koyo</t>
+  </si>
+  <si>
     <t>Ultrafix 5 cm x 1 m</t>
   </si>
   <si>
-    <t>Asam mefenamat</t>
-  </si>
-  <si>
-    <t>Charm wings</t>
-  </si>
-  <si>
-    <t>Hansaplast koyo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gelang tangan DNR </t>
   </si>
   <si>
+    <t>Sarung tangan Uk M</t>
+  </si>
+  <si>
     <t xml:space="preserve">Verban 10 cm </t>
   </si>
   <si>
-    <t>Sarung tangan Uk M</t>
-  </si>
-  <si>
     <t xml:space="preserve">Threeway </t>
   </si>
   <si>
@@ -125,18 +125,18 @@
     <t>Spuit 50cc</t>
   </si>
   <si>
+    <t xml:space="preserve">Ambroxol </t>
+  </si>
+  <si>
+    <t>Diapet</t>
+  </si>
+  <si>
     <t>Spuit 10 cc</t>
   </si>
   <si>
-    <t xml:space="preserve">Ambroxol </t>
-  </si>
-  <si>
     <t>Gelang tangan dewasa perempuan</t>
   </si>
   <si>
-    <t>Diapet</t>
-  </si>
-  <si>
     <t>Urine bag</t>
   </si>
   <si>
@@ -155,27 +155,30 @@
     <t>Selang suction</t>
   </si>
   <si>
+    <t xml:space="preserve">Selang NGT </t>
+  </si>
+  <si>
     <t xml:space="preserve">Spuit 20 </t>
   </si>
   <si>
     <t>Sarung tangan panjang sterill</t>
   </si>
   <si>
-    <t xml:space="preserve">Selang NGT </t>
-  </si>
-  <si>
     <t>Heacting set</t>
   </si>
   <si>
     <t xml:space="preserve">Ventolyn </t>
   </si>
   <si>
+    <t xml:space="preserve">Aquades </t>
+  </si>
+  <si>
+    <t>Gelang tangan anak laki-laki</t>
+  </si>
+  <si>
     <t>NaCl 500ml</t>
   </si>
   <si>
-    <t>Gelang tangan anak laki-laki</t>
-  </si>
-  <si>
     <t>Selang OGT</t>
   </si>
   <si>
@@ -194,6 +197,9 @@
     <t xml:space="preserve">Sabun cuci Kimia </t>
   </si>
   <si>
+    <t>Extention tube</t>
+  </si>
+  <si>
     <t xml:space="preserve">Masker nebulizer </t>
   </si>
   <si>
@@ -212,12 +218,6 @@
     <t>Wool</t>
   </si>
   <si>
-    <t xml:space="preserve">Aquades </t>
-  </si>
-  <si>
-    <t>Extention tube</t>
-  </si>
-  <si>
     <t xml:space="preserve">Foam dressing </t>
   </si>
   <si>
@@ -236,6 +236,15 @@
     <t>Smart garlic wound zalf</t>
   </si>
   <si>
+    <t>Alginate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allevyn </t>
+  </si>
+  <si>
+    <t>Betaplast</t>
+  </si>
+  <si>
     <t>Excle care hydrosoloid</t>
   </si>
   <si>
@@ -245,6 +254,9 @@
     <t>Indosorb</t>
   </si>
   <si>
+    <t xml:space="preserve">Inomed foam </t>
+  </si>
+  <si>
     <t>Kilbac</t>
   </si>
   <si>
@@ -285,18 +297,6 @@
   </si>
   <si>
     <t xml:space="preserve">W care AH </t>
-  </si>
-  <si>
-    <t>Alginate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allevyn </t>
-  </si>
-  <si>
-    <t>Betaplast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inomed foam </t>
   </si>
 </sst>
 </file>
@@ -702,13 +702,13 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>1389</v>
+        <v>1400</v>
       </c>
       <c r="E3">
         <v>150</v>
       </c>
       <c r="F3">
-        <v>208350</v>
+        <v>210000</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -722,13 +722,13 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="E4">
         <v>200</v>
       </c>
       <c r="F4">
-        <v>179600</v>
+        <v>180000</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -902,13 +902,13 @@
         <v>17</v>
       </c>
       <c r="D13">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E13">
         <v>400</v>
       </c>
       <c r="F13">
-        <v>31600</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1016,7 +1016,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -1025,10 +1025,10 @@
         <v>60</v>
       </c>
       <c r="E19">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="F19">
-        <v>24000</v>
+        <v>21000</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1036,7 +1036,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
@@ -1045,10 +1045,10 @@
         <v>60</v>
       </c>
       <c r="E20">
-        <v>4200</v>
+        <v>900</v>
       </c>
       <c r="F20">
-        <v>252000</v>
+        <v>54000</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1056,19 +1056,19 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
       </c>
       <c r="D21">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E21">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="F21">
-        <v>20650</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1076,19 +1076,19 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
       </c>
       <c r="D22">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E22">
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="F22">
-        <v>53100</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1096,19 +1096,19 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
       </c>
       <c r="D23">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E23">
-        <v>750</v>
+        <v>4200</v>
       </c>
       <c r="F23">
-        <v>43500</v>
+        <v>252000</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1136,7 +1136,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -1145,10 +1145,10 @@
         <v>50</v>
       </c>
       <c r="E25">
-        <v>1100</v>
+        <v>980</v>
       </c>
       <c r="F25">
-        <v>55000</v>
+        <v>49000</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1156,19 +1156,19 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
       </c>
       <c r="D26">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E26">
-        <v>980</v>
+        <v>1100</v>
       </c>
       <c r="F26">
-        <v>47040</v>
+        <v>55000</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1276,7 +1276,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
         <v>36</v>
@@ -1285,10 +1285,10 @@
         <v>30</v>
       </c>
       <c r="E32">
-        <v>4000</v>
+        <v>300</v>
       </c>
       <c r="F32">
-        <v>120000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1296,19 +1296,19 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
       </c>
       <c r="D33">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E33">
         <v>300</v>
       </c>
       <c r="F33">
-        <v>8700</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1316,19 +1316,19 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
       </c>
       <c r="D34">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E34">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="F34">
-        <v>29000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1336,19 +1336,19 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
         <v>39</v>
       </c>
       <c r="D35">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E35">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="F35">
-        <v>8400</v>
+        <v>29000</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1476,7 +1476,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
         <v>46</v>
@@ -1485,10 +1485,10 @@
         <v>16</v>
       </c>
       <c r="E42">
-        <v>8000</v>
+        <v>29500</v>
       </c>
       <c r="F42">
-        <v>128000</v>
+        <v>472000</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1496,19 +1496,19 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
         <v>47</v>
       </c>
       <c r="D43">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E43">
-        <v>20000</v>
+        <v>8000</v>
       </c>
       <c r="F43">
-        <v>300000</v>
+        <v>128000</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1516,7 +1516,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
         <v>48</v>
@@ -1525,10 +1525,10 @@
         <v>15</v>
       </c>
       <c r="E44">
-        <v>29500</v>
+        <v>20000</v>
       </c>
       <c r="F44">
-        <v>442500</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1576,7 +1576,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
         <v>51</v>
@@ -1602,13 +1602,13 @@
         <v>52</v>
       </c>
       <c r="D48">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E48">
         <v>800</v>
       </c>
       <c r="F48">
-        <v>6400</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1616,19 +1616,19 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C49" t="s">
         <v>53</v>
       </c>
       <c r="D49">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E49">
-        <v>17500</v>
+        <v>13000</v>
       </c>
       <c r="F49">
-        <v>122500</v>
+        <v>117000</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1636,19 +1636,19 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C50" t="s">
         <v>54</v>
       </c>
       <c r="D50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E50">
-        <v>27000</v>
+        <v>17500</v>
       </c>
       <c r="F50">
-        <v>162000</v>
+        <v>122500</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1656,7 +1656,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C51" t="s">
         <v>55</v>
@@ -1665,10 +1665,10 @@
         <v>6</v>
       </c>
       <c r="E51">
-        <v>11000</v>
+        <v>27000</v>
       </c>
       <c r="F51">
-        <v>66000</v>
+        <v>162000</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1676,19 +1676,19 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
         <v>56</v>
       </c>
       <c r="D52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E52">
-        <v>9500</v>
+        <v>11000</v>
       </c>
       <c r="F52">
-        <v>47500</v>
+        <v>66000</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1696,7 +1696,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
         <v>57</v>
@@ -1705,10 +1705,10 @@
         <v>5</v>
       </c>
       <c r="E53">
-        <v>800</v>
+        <v>9500</v>
       </c>
       <c r="F53">
-        <v>4000</v>
+        <v>47500</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1716,7 +1716,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
         <v>58</v>
@@ -1725,10 +1725,10 @@
         <v>5</v>
       </c>
       <c r="E54">
-        <v>15000</v>
+        <v>800</v>
       </c>
       <c r="F54">
-        <v>75000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1736,19 +1736,19 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C55" t="s">
         <v>59</v>
       </c>
       <c r="D55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E55">
-        <v>9000</v>
+        <v>15000</v>
       </c>
       <c r="F55">
-        <v>36000</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1756,7 +1756,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="C56" t="s">
         <v>60</v>
@@ -1765,10 +1765,10 @@
         <v>4</v>
       </c>
       <c r="E56">
-        <v>32000</v>
+        <v>12487</v>
       </c>
       <c r="F56">
-        <v>128000</v>
+        <v>49948</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1776,19 +1776,19 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s">
         <v>61</v>
       </c>
       <c r="D57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E57">
-        <v>125000</v>
+        <v>9000</v>
       </c>
       <c r="F57">
-        <v>375000</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1796,19 +1796,19 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="C58" t="s">
         <v>62</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E58">
-        <v>16000</v>
+        <v>32000</v>
       </c>
       <c r="F58">
-        <v>48000</v>
+        <v>128000</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1816,7 +1816,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
         <v>63</v>
@@ -1825,10 +1825,10 @@
         <v>3</v>
       </c>
       <c r="E59">
-        <v>9500</v>
+        <v>125000</v>
       </c>
       <c r="F59">
-        <v>28500</v>
+        <v>375000</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1836,7 +1836,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="C60" t="s">
         <v>64</v>
@@ -1845,10 +1845,10 @@
         <v>3</v>
       </c>
       <c r="E60">
-        <v>40000</v>
+        <v>16000</v>
       </c>
       <c r="F60">
-        <v>120000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1856,19 +1856,19 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C61" t="s">
         <v>65</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E61">
-        <v>13000</v>
+        <v>9500</v>
       </c>
       <c r="F61">
-        <v>26000</v>
+        <v>28500</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1876,19 +1876,19 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="C62" t="s">
         <v>66</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E62">
-        <v>12487</v>
+        <v>40000</v>
       </c>
       <c r="F62">
-        <v>24974</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2016,7 +2016,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C69" t="s">
         <v>73</v>
@@ -2036,7 +2036,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
         <v>74</v>
@@ -2045,10 +2045,10 @@
         <v>1</v>
       </c>
       <c r="E70">
-        <v>130000</v>
+        <v>125000</v>
       </c>
       <c r="F70">
-        <v>130000</v>
+        <v>125000</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2056,7 +2056,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C71" t="s">
         <v>75</v>
@@ -2065,10 +2065,10 @@
         <v>1</v>
       </c>
       <c r="E71">
-        <v>100000</v>
+        <v>40000</v>
       </c>
       <c r="F71">
-        <v>100000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2076,7 +2076,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C72" t="s">
         <v>76</v>
@@ -2085,10 +2085,10 @@
         <v>1</v>
       </c>
       <c r="E72">
-        <v>32000</v>
+        <v>50000</v>
       </c>
       <c r="F72">
-        <v>32000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2096,7 +2096,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C73" t="s">
         <v>77</v>
@@ -2105,10 +2105,10 @@
         <v>1</v>
       </c>
       <c r="E73">
-        <v>175000</v>
+        <v>130000</v>
       </c>
       <c r="F73">
-        <v>175000</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2116,7 +2116,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C74" t="s">
         <v>78</v>
@@ -2125,10 +2125,10 @@
         <v>1</v>
       </c>
       <c r="E74">
-        <v>15000</v>
+        <v>100000</v>
       </c>
       <c r="F74">
-        <v>15000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2136,7 +2136,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C75" t="s">
         <v>79</v>
@@ -2145,10 +2145,10 @@
         <v>1</v>
       </c>
       <c r="E75">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="F75">
-        <v>40000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2156,7 +2156,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C76" t="s">
         <v>80</v>
@@ -2165,10 +2165,10 @@
         <v>1</v>
       </c>
       <c r="E76">
-        <v>50000</v>
+        <v>32000</v>
       </c>
       <c r="F76">
-        <v>50000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2176,7 +2176,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C77" t="s">
         <v>81</v>
@@ -2185,10 +2185,10 @@
         <v>1</v>
       </c>
       <c r="E77">
-        <v>80000</v>
+        <v>175000</v>
       </c>
       <c r="F77">
-        <v>80000</v>
+        <v>175000</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2196,7 +2196,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C78" t="s">
         <v>82</v>
@@ -2205,10 +2205,10 @@
         <v>1</v>
       </c>
       <c r="E78">
-        <v>85000</v>
+        <v>15000</v>
       </c>
       <c r="F78">
-        <v>85000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2216,7 +2216,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C79" t="s">
         <v>83</v>
@@ -2225,10 +2225,10 @@
         <v>1</v>
       </c>
       <c r="E79">
-        <v>250000</v>
+        <v>40000</v>
       </c>
       <c r="F79">
-        <v>250000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2236,7 +2236,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="C80" t="s">
         <v>84</v>
@@ -2245,10 +2245,10 @@
         <v>1</v>
       </c>
       <c r="E80">
-        <v>70000</v>
+        <v>50000</v>
       </c>
       <c r="F80">
-        <v>70000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2256,7 +2256,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C81" t="s">
         <v>85</v>
@@ -2265,10 +2265,10 @@
         <v>1</v>
       </c>
       <c r="E81">
-        <v>25000</v>
+        <v>80000</v>
       </c>
       <c r="F81">
-        <v>25000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2276,7 +2276,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C82" t="s">
         <v>86</v>
@@ -2285,10 +2285,10 @@
         <v>1</v>
       </c>
       <c r="E82">
-        <v>12000</v>
+        <v>85000</v>
       </c>
       <c r="F82">
-        <v>12000</v>
+        <v>85000</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2296,7 +2296,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C83" t="s">
         <v>87</v>
@@ -2305,10 +2305,10 @@
         <v>1</v>
       </c>
       <c r="E83">
-        <v>45000</v>
+        <v>250000</v>
       </c>
       <c r="F83">
-        <v>45000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2316,7 +2316,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C84" t="s">
         <v>88</v>
@@ -2325,10 +2325,10 @@
         <v>1</v>
       </c>
       <c r="E84">
-        <v>45000</v>
+        <v>70000</v>
       </c>
       <c r="F84">
-        <v>45000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2336,7 +2336,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C85" t="s">
         <v>89</v>
@@ -2345,10 +2345,10 @@
         <v>1</v>
       </c>
       <c r="E85">
-        <v>75000</v>
+        <v>25000</v>
       </c>
       <c r="F85">
-        <v>75000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2356,19 +2356,19 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="C86" t="s">
         <v>90</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86">
-        <v>50000</v>
+        <v>12000</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2376,19 +2376,19 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="C87" t="s">
         <v>91</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87">
-        <v>125000</v>
+        <v>45000</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2396,19 +2396,19 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="C88" t="s">
         <v>92</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E88">
-        <v>40000</v>
+        <v>45000</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2416,19 +2416,19 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="C89" t="s">
         <v>93</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E89">
-        <v>50000</v>
+        <v>75000</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>75000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>